<commit_message>
admin-order (search, excel, status). update(cart, checkout)
</commit_message>
<xml_diff>
--- a/Orders.xlsx
+++ b/Orders.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>STT</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>00:00:00 10/06/2024</t>
-  </si>
-  <si>
-    <t>09:56:37 11/06/2024</t>
   </si>
   <si>
     <t>Nguyễn Thị Diệu Mỵ</t>
@@ -131,7 +128,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -174,7 +171,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="n" s="0">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="C2" t="s" s="0">
         <v>7</v>
@@ -189,7 +186,7 @@
         <v>0.0</v>
       </c>
       <c r="G2" t="n" s="0">
-        <v>4389000.0</v>
+        <v>1.32389E8</v>
       </c>
     </row>
     <row r="3">
@@ -197,22 +194,22 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n" s="2">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s" s="2">
         <v>8</v>
       </c>
       <c r="E3" t="s" s="2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F3" t="n" s="2">
         <v>0.0</v>
       </c>
       <c r="G3" t="n" s="2">
-        <v>1.32389E8</v>
+        <v>8994000.0</v>
       </c>
     </row>
     <row r="4">
@@ -220,22 +217,22 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n" s="0">
-        <v>7.0</v>
+        <v>9.0</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s" s="0">
         <v>8</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F4" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="G4" t="n" s="0">
-        <v>2190000.0</v>
+        <v>8.3098E7</v>
       </c>
     </row>
     <row r="5">
@@ -243,67 +240,21 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n" s="2">
-        <v>8.0</v>
+        <v>10.0</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s" s="2">
         <v>8</v>
       </c>
       <c r="E5" t="s" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F5" t="n" s="2">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="G5" t="n" s="2">
-        <v>8994000.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n" s="0">
-        <v>5.0</v>
-      </c>
-      <c r="B6" t="n" s="0">
-        <v>9.0</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="F6" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="G6" t="n" s="0">
-        <v>8.3098E7</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B7" t="n" s="2">
-        <v>10.0</v>
-      </c>
-      <c r="C7" t="s" s="2">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s" s="2">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s" s="2">
-        <v>15</v>
-      </c>
-      <c r="F7" t="n" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="G7" t="n" s="2">
         <v>6.7799E7</v>
       </c>
     </row>

</xml_diff>